<commit_message>
Update LP excel Cal
</commit_message>
<xml_diff>
--- a/_Excel/LP.xlsx
+++ b/_Excel/LP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bridge\City2223_SEM_A\EE3301\letcure\edit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39470999-C743-4125-A714-620E95F2B192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55ABBF-1B3F-4F47-9FCD-DB53974E0AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2025" windowWidth="21600" windowHeight="13305" firstSheet="1" activeTab="2" xr2:uid="{DA5D110B-5606-4367-BCF8-9589C927E560}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{DA5D110B-5606-4367-BCF8-9589C927E560}"/>
   </bookViews>
   <sheets>
     <sheet name="LP" sheetId="1" r:id="rId1"/>
@@ -19,220 +19,301 @@
     <sheet name="LP Mat UV" sheetId="5" r:id="rId4"/>
     <sheet name="Dual" sheetId="6" r:id="rId5"/>
     <sheet name="Convex  Opt." sheetId="7" r:id="rId6"/>
+    <sheet name="Knapsack LP" sheetId="10" r:id="rId7"/>
+    <sheet name="Knapsack ILP" sheetId="8" r:id="rId8"/>
+    <sheet name="Knapsack Greedy" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="5" hidden="1">'Convex  Opt.'!$A$11:$C$11</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">Dual!$C$39:$L$39</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'Knapsack ILP'!$C$9:$L$9</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'Knapsack LP'!$C$19:$L$19</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">LP!$E$11:$G$11</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'LP Mat'!$C$23:$L$23</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'LP Mat UV'!$C$23:$L$24</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'LP UV'!$E$11:$K$11</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs0" localSheetId="7" hidden="1">'Knapsack ILP'!$O$3:$O$3</definedName>
     <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Convex  Opt.'!$A$11:$C$11</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">Dual!$O$24:$O$33</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'Knapsack ILP'!$O$3</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Knapsack LP'!$C$19:$L$19</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">LP!$F$3:$F$7</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'LP Mat'!$C$23:$L$23</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'LP Mat UV'!$O$13:$O$17</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'LP UV'!$F$3:$F$7</definedName>
     <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Convex  Opt.'!$F$3:$F$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">'Knapsack ILP'!$C$9:$L$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'Knapsack LP'!$O$3:$O$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">LP!$M$3:$M$7</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'LP Mat'!$O$13:$O$17</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'LP Mat UV'!$O$3:$O$7</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'LP UV'!$M$3:$M$7</definedName>
     <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Convex  Opt.'!$M$3:$M$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="7" hidden="1">'Knapsack ILP'!$O$3:$O$3</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">LP!$M$3:$M$7</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'LP Mat'!$O$3:$O$7</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'LP Mat UV'!$O$8:$O$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="7" hidden="1">'Knapsack ILP'!#REF!</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'LP Mat'!$O$8:$O$12</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'LP Mat'!$O$9:$O$13</definedName>
     <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="5" hidden="1">'Convex  Opt.'!$E$11</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">Dual!$N$39</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Knapsack ILP'!$N$9</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'Knapsack LP'!$N$19</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">LP!$H$11</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'LP Mat'!$N$23</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'LP Mat UV'!$N$23</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'LP UV'!$L$11</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel0" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="5" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs0" localSheetId="7" hidden="1">'Knapsack ILP'!$N$3:$N$3</definedName>
     <definedName name="solver_rhs1" localSheetId="5" hidden="1">"整數"</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">Dual!$N$24:$N$33</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">'Knapsack ILP'!$N$3</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">"整數"</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">LP!$E$3:$E$7</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">"整數"</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">'LP Mat UV'!$N$13:$N$17</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'LP UV'!$E$3:$E$7</definedName>
     <definedName name="solver_rhs2" localSheetId="5" hidden="1">'Convex  Opt.'!$E$3:$E$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">"二進制"</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">'Knapsack LP'!$N$3:$N$13</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">LP!$L$3:$L$7</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'LP Mat'!$N$13:$N$17</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">'LP Mat UV'!$N$3:$N$7</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'LP UV'!$L$3:$L$7</definedName>
     <definedName name="solver_rhs3" localSheetId="5" hidden="1">'Convex  Opt.'!$L$3:$L$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="7" hidden="1">'Knapsack ILP'!$N$3:$N$3</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">LP!$L$3:$L$7</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'LP Mat'!$N$3:$N$7</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">'LP Mat UV'!$N$8:$N$12</definedName>
+    <definedName name="solver_rhs4" localSheetId="7" hidden="1">'Knapsack ILP'!#REF!</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'LP Mat'!$N$8:$N$12</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">'LP Mat'!$N$9:$N$13</definedName>
     <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -250,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="86">
   <si>
     <t>Subject to</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -528,12 +609,78 @@
     <t>Diff</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Unsort</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi/wi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>W remain</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (You need to sort the table by yourself)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -593,6 +740,14 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -632,7 +787,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="87">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -1754,13 +1909,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2193,6 +2428,72 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="87" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="89" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="87" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="89" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="87" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2223,18 +2524,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2244,6 +2545,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2259,12 +2566,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2272,13 +2573,152 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2687,21 +3127,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="146"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="168"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -2889,16 +3329,16 @@
     </row>
     <row r="8" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="147" t="s">
+      <c r="A9" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="149"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="171"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -2974,21 +3414,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="146"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="168"/>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -3180,24 +3620,24 @@
     </row>
     <row r="8" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="147" t="s">
+      <c r="A9" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="149"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="170"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="170"/>
+      <c r="M9" s="170"/>
+      <c r="N9" s="170"/>
+      <c r="O9" s="170"/>
+      <c r="P9" s="171"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -3309,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825411DF-E3DB-4E9F-8A6D-BFA9AC4C91BF}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3325,29 +3765,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="146"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="168"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="176" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="151"/>
+      <c r="B2" s="173"/>
       <c r="C2" s="41" t="s">
         <v>8</v>
       </c>
@@ -3389,19 +3829,19 @@
       <c r="A3" s="122"/>
       <c r="B3" s="46"/>
       <c r="C3" s="56">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" s="57">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E3" s="57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="57">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="57">
         <v>0</v>
@@ -3422,21 +3862,21 @@
         <v>1</v>
       </c>
       <c r="N3" s="68">
-        <v>2400</v>
+        <v>6</v>
       </c>
       <c r="O3" s="95">
         <f t="array" ref="O3">MMULT(C3:L3,TRANSPOSE(C$23:L$23))</f>
-        <v>2400</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" s="49"/>
       <c r="C4" s="59">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="60">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="60">
         <v>0</v>
@@ -3466,11 +3906,11 @@
         <v>1</v>
       </c>
       <c r="N4" s="69">
-        <v>2280</v>
+        <v>0</v>
       </c>
       <c r="O4" s="97">
         <f t="array" ref="O4">MMULT(C4:L4,TRANSPOSE(C$23:L$23))</f>
-        <v>2275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3612,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="57">
         <v>0</v>
@@ -3642,11 +4082,11 @@
         <v>3</v>
       </c>
       <c r="N8" s="68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O8" s="95">
         <f t="array" ref="O8">MMULT(C8:L8,TRANSPOSE(C$23:L$23))</f>
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4046,26 +4486,26 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
-      <c r="H19" s="157"/>
-      <c r="I19" s="157"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="151"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="177"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="177"/>
+      <c r="L19" s="177"/>
+      <c r="M19" s="177"/>
+      <c r="N19" s="173"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="154"/>
-      <c r="B20" s="155"/>
+      <c r="A20" s="178"/>
+      <c r="B20" s="179"/>
       <c r="C20" s="45" t="s">
         <v>47</v>
       </c>
@@ -4100,24 +4540,24 @@
       <c r="N20" s="46"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="150" t="s">
+      <c r="A21" s="172" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="151"/>
+      <c r="B21" s="173"/>
       <c r="C21" s="74">
-        <v>4.983333</v>
+        <v>4</v>
       </c>
       <c r="D21" s="75">
-        <v>6.7166670000000002</v>
+        <v>2</v>
       </c>
       <c r="E21" s="75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21" s="75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G21" s="75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="75">
         <v>0</v>
@@ -4138,8 +4578,8 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
-      <c r="B22" s="153"/>
+      <c r="A22" s="174"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="41" t="s">
         <v>8</v>
       </c>
@@ -4176,15 +4616,15 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="150" t="s">
+      <c r="A23" s="172" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="151"/>
+      <c r="B23" s="173"/>
       <c r="C23" s="85">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="D23" s="86">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="E23" s="86">
         <v>0</v>
@@ -4213,7 +4653,7 @@
       <c r="M23" s="53"/>
       <c r="N23" s="88">
         <f t="array" ref="N23">MMULT(C21:L21,TRANSPOSE(C$23:L$23))</f>
-        <v>1757.1666719999998</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -4270,23 +4710,23 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:L17">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21 C23:L23">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4314,29 +4754,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="146"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="168"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="155"/>
+      <c r="B2" s="179"/>
       <c r="C2" s="41" t="s">
         <v>8</v>
       </c>
@@ -5035,26 +5475,26 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
-      <c r="H19" s="157"/>
-      <c r="I19" s="157"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="151"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="177"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="177"/>
+      <c r="L19" s="177"/>
+      <c r="M19" s="177"/>
+      <c r="N19" s="173"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="154"/>
-      <c r="B20" s="155"/>
+      <c r="A20" s="178"/>
+      <c r="B20" s="179"/>
       <c r="C20" s="45" t="s">
         <v>47</v>
       </c>
@@ -5089,10 +5529,10 @@
       <c r="N20" s="49"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="150" t="s">
+      <c r="A21" s="172" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="151"/>
+      <c r="B21" s="173"/>
       <c r="C21" s="74">
         <v>7</v>
       </c>
@@ -5127,8 +5567,8 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
-      <c r="B22" s="153"/>
+      <c r="A22" s="174"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="42" t="s">
         <v>8</v>
       </c>
@@ -5165,10 +5605,10 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="154" t="s">
+      <c r="A23" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="155"/>
+      <c r="B23" s="179"/>
       <c r="C23" s="77">
         <v>5</v>
       </c>
@@ -5206,10 +5646,10 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="158" t="s">
+      <c r="A24" s="180" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="159"/>
+      <c r="B24" s="181"/>
       <c r="C24" s="81">
         <v>0</v>
       </c>
@@ -5256,12 +5696,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:L17 C21:L21 C23:L24">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N17">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5293,48 +5733,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="185" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="162"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="186"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="145"/>
-      <c r="M2" s="145"/>
-      <c r="N2" s="145"/>
-      <c r="O2" s="146"/>
+      <c r="A2" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="168"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="176" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="151"/>
+      <c r="B3" s="173"/>
       <c r="C3" s="41" t="s">
         <v>8</v>
       </c>
@@ -5813,26 +6253,26 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="150" t="s">
+      <c r="A15" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="157"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="157"/>
-      <c r="J15" s="157"/>
-      <c r="K15" s="157"/>
-      <c r="L15" s="157"/>
-      <c r="M15" s="157"/>
-      <c r="N15" s="151"/>
+      <c r="B15" s="177"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="177"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="177"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="177"/>
+      <c r="N15" s="173"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="150"/>
-      <c r="B16" s="151"/>
+      <c r="A16" s="172"/>
+      <c r="B16" s="173"/>
       <c r="C16" s="45" t="s">
         <v>47</v>
       </c>
@@ -5867,10 +6307,10 @@
       <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="150" t="s">
+      <c r="A17" s="172" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="151"/>
+      <c r="B17" s="173"/>
       <c r="C17" s="74">
         <v>4.2999999999999997E-2</v>
       </c>
@@ -5905,8 +6345,8 @@
       <c r="N17" s="49"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="151"/>
+      <c r="A18" s="172"/>
+      <c r="B18" s="173"/>
       <c r="C18" s="41" t="s">
         <v>8</v>
       </c>
@@ -5943,10 +6383,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="172" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="151"/>
+      <c r="B19" s="173"/>
       <c r="C19" s="85">
         <v>2.1818181818181817</v>
       </c>
@@ -6000,48 +6440,48 @@
       <c r="N20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="163" t="s">
+      <c r="A21" s="187" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="164"/>
-      <c r="C21" s="164"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
-      <c r="F21" s="164"/>
-      <c r="G21" s="164"/>
-      <c r="H21" s="164"/>
-      <c r="I21" s="164"/>
-      <c r="J21" s="164"/>
-      <c r="K21" s="164"/>
-      <c r="L21" s="164"/>
-      <c r="M21" s="164"/>
-      <c r="N21" s="164"/>
-      <c r="O21" s="165"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
+      <c r="D21" s="188"/>
+      <c r="E21" s="188"/>
+      <c r="F21" s="188"/>
+      <c r="G21" s="188"/>
+      <c r="H21" s="188"/>
+      <c r="I21" s="188"/>
+      <c r="J21" s="188"/>
+      <c r="K21" s="188"/>
+      <c r="L21" s="188"/>
+      <c r="M21" s="188"/>
+      <c r="N21" s="188"/>
+      <c r="O21" s="189"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="145"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="145"/>
-      <c r="F22" s="145"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="145"/>
-      <c r="J22" s="145"/>
-      <c r="K22" s="145"/>
-      <c r="L22" s="145"/>
-      <c r="M22" s="145"/>
-      <c r="N22" s="145"/>
-      <c r="O22" s="146"/>
+      <c r="A22" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="167"/>
+      <c r="C22" s="167"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="167"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="167"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="167"/>
+      <c r="M22" s="167"/>
+      <c r="N22" s="167"/>
+      <c r="O22" s="168"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="156" t="s">
+      <c r="A23" s="176" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="151"/>
+      <c r="B23" s="173"/>
       <c r="C23" s="41" t="s">
         <v>58</v>
       </c>
@@ -6523,27 +6963,27 @@
     </row>
     <row r="34" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="144" t="s">
+      <c r="A35" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="145"/>
-      <c r="C35" s="145"/>
-      <c r="D35" s="145"/>
-      <c r="E35" s="145"/>
-      <c r="F35" s="145"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="145"/>
-      <c r="I35" s="145"/>
-      <c r="J35" s="145"/>
-      <c r="K35" s="145"/>
-      <c r="L35" s="145"/>
-      <c r="M35" s="145"/>
-      <c r="N35" s="145"/>
-      <c r="O35" s="146"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="167"/>
+      <c r="J35" s="167"/>
+      <c r="K35" s="167"/>
+      <c r="L35" s="167"/>
+      <c r="M35" s="167"/>
+      <c r="N35" s="167"/>
+      <c r="O35" s="168"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="156"/>
-      <c r="B36" s="151"/>
+      <c r="A36" s="176"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="45" t="s">
         <v>30</v>
       </c>
@@ -6579,10 +7019,10 @@
       <c r="O36" s="135"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="151"/>
+      <c r="B37" s="173"/>
       <c r="C37" s="85">
         <f t="array" ref="C37:L37">TRANSPOSE(N4:N13)</f>
         <v>10</v>
@@ -6619,8 +7059,8 @@
       <c r="O37" s="136"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="156"/>
-      <c r="B38" s="151"/>
+      <c r="A38" s="176"/>
+      <c r="B38" s="173"/>
       <c r="C38" s="41" t="s">
         <v>58</v>
       </c>
@@ -6660,10 +7100,10 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="166" t="s">
+      <c r="A39" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="167"/>
+      <c r="B39" s="184"/>
       <c r="C39" s="137">
         <v>2.9836363636363637E-2</v>
       </c>
@@ -6706,6 +7146,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:O22"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A17:B17"/>
@@ -6717,40 +7162,35 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A21:O21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:O22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C4:L13">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:L17 C19:L19">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:L37 C39:L39">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:L33">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24:N33">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6773,21 +7213,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="146"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="168"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -6981,16 +7421,16 @@
     </row>
     <row r="8" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="147" t="s">
+      <c r="A9" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="149"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="171"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -7025,11 +7465,11 @@
         <f>5.5*A11+7.5*B11-3*(7*A11+9*B11)/60-2*(5*A11+10*B11)/60</f>
         <v>1757.1666666666667</v>
       </c>
-      <c r="F11" s="168" t="s">
+      <c r="F11" s="190" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="169"/>
-      <c r="H11" s="170"/>
+      <c r="G11" s="191"/>
+      <c r="H11" s="192"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
@@ -7042,4 +7482,1488 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7ED2B1-ED26-48D8-A59A-8352A325EF80}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="41" customWidth="1"/>
+    <col min="3" max="12" width="9" style="41"/>
+    <col min="13" max="13" width="2.625" style="41" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="41" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="168"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="176" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="173"/>
+      <c r="C2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="122"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="56">
+        <v>2</v>
+      </c>
+      <c r="D3" s="57">
+        <v>1</v>
+      </c>
+      <c r="E3" s="57">
+        <v>3</v>
+      </c>
+      <c r="F3" s="57">
+        <v>3</v>
+      </c>
+      <c r="G3" s="57">
+        <v>2</v>
+      </c>
+      <c r="H3" s="57">
+        <v>1</v>
+      </c>
+      <c r="I3" s="57">
+        <v>0</v>
+      </c>
+      <c r="J3" s="57">
+        <v>0</v>
+      </c>
+      <c r="K3" s="57">
+        <v>0</v>
+      </c>
+      <c r="L3" s="58">
+        <v>0</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="68">
+        <v>8</v>
+      </c>
+      <c r="O3" s="95">
+        <f t="array" ref="O3">MMULT(C3:L3,TRANSPOSE(C$19:L$19))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="59">
+        <v>1</v>
+      </c>
+      <c r="D4" s="60">
+        <v>0</v>
+      </c>
+      <c r="E4" s="60">
+        <v>0</v>
+      </c>
+      <c r="F4" s="60">
+        <v>0</v>
+      </c>
+      <c r="G4" s="60">
+        <v>0</v>
+      </c>
+      <c r="H4" s="60">
+        <v>0</v>
+      </c>
+      <c r="I4" s="60">
+        <v>0</v>
+      </c>
+      <c r="J4" s="60">
+        <v>0</v>
+      </c>
+      <c r="K4" s="60">
+        <v>0</v>
+      </c>
+      <c r="L4" s="61">
+        <v>0</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="69">
+        <v>1</v>
+      </c>
+      <c r="O4" s="97">
+        <f t="array" ref="O4">MMULT(C4:L4,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="59">
+        <v>0</v>
+      </c>
+      <c r="D5" s="60">
+        <v>1</v>
+      </c>
+      <c r="E5" s="60">
+        <v>0</v>
+      </c>
+      <c r="F5" s="60">
+        <v>0</v>
+      </c>
+      <c r="G5" s="60">
+        <v>0</v>
+      </c>
+      <c r="H5" s="60">
+        <v>0</v>
+      </c>
+      <c r="I5" s="60">
+        <v>0</v>
+      </c>
+      <c r="J5" s="60">
+        <v>0</v>
+      </c>
+      <c r="K5" s="60">
+        <v>0</v>
+      </c>
+      <c r="L5" s="61">
+        <v>0</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="69">
+        <v>1</v>
+      </c>
+      <c r="O5" s="97">
+        <f t="array" ref="O5">MMULT(C5:L5,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="59">
+        <v>0</v>
+      </c>
+      <c r="D6" s="60">
+        <v>0</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="F6" s="60">
+        <v>0</v>
+      </c>
+      <c r="G6" s="60">
+        <v>0</v>
+      </c>
+      <c r="H6" s="60">
+        <v>0</v>
+      </c>
+      <c r="I6" s="60">
+        <v>0</v>
+      </c>
+      <c r="J6" s="60">
+        <v>0</v>
+      </c>
+      <c r="K6" s="60">
+        <v>0</v>
+      </c>
+      <c r="L6" s="61">
+        <v>0</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="69">
+        <v>1</v>
+      </c>
+      <c r="O6" s="97">
+        <f t="array" ref="O6">MMULT(C6:L6,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="59">
+        <v>0</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0</v>
+      </c>
+      <c r="E7" s="60">
+        <v>0</v>
+      </c>
+      <c r="F7" s="60">
+        <v>1</v>
+      </c>
+      <c r="G7" s="60">
+        <v>0</v>
+      </c>
+      <c r="H7" s="60">
+        <v>0</v>
+      </c>
+      <c r="I7" s="60">
+        <v>0</v>
+      </c>
+      <c r="J7" s="60">
+        <v>0</v>
+      </c>
+      <c r="K7" s="60">
+        <v>0</v>
+      </c>
+      <c r="L7" s="61">
+        <v>0</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="69">
+        <v>1</v>
+      </c>
+      <c r="O7" s="97">
+        <f t="array" ref="O7">MMULT(C7:L7,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="59">
+        <v>0</v>
+      </c>
+      <c r="D8" s="60">
+        <v>0</v>
+      </c>
+      <c r="E8" s="60">
+        <v>0</v>
+      </c>
+      <c r="F8" s="60">
+        <v>0</v>
+      </c>
+      <c r="G8" s="60">
+        <v>1</v>
+      </c>
+      <c r="H8" s="60">
+        <v>0</v>
+      </c>
+      <c r="I8" s="60">
+        <v>0</v>
+      </c>
+      <c r="J8" s="60">
+        <v>0</v>
+      </c>
+      <c r="K8" s="60">
+        <v>0</v>
+      </c>
+      <c r="L8" s="61">
+        <v>0</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="69">
+        <v>1</v>
+      </c>
+      <c r="O8" s="97">
+        <f t="array" ref="O8">MMULT(C8:L8,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="59">
+        <v>0</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0</v>
+      </c>
+      <c r="E9" s="60">
+        <v>0</v>
+      </c>
+      <c r="F9" s="60">
+        <v>0</v>
+      </c>
+      <c r="G9" s="60">
+        <v>0</v>
+      </c>
+      <c r="H9" s="60">
+        <v>1</v>
+      </c>
+      <c r="I9" s="60">
+        <v>0</v>
+      </c>
+      <c r="J9" s="60">
+        <v>0</v>
+      </c>
+      <c r="K9" s="60">
+        <v>0</v>
+      </c>
+      <c r="L9" s="61">
+        <v>0</v>
+      </c>
+      <c r="M9" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="69">
+        <v>1</v>
+      </c>
+      <c r="O9" s="97">
+        <f t="array" ref="O9">MMULT(C9:L9,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="59">
+        <v>0</v>
+      </c>
+      <c r="D10" s="60">
+        <v>0</v>
+      </c>
+      <c r="E10" s="60">
+        <v>0</v>
+      </c>
+      <c r="F10" s="60">
+        <v>0</v>
+      </c>
+      <c r="G10" s="60">
+        <v>0</v>
+      </c>
+      <c r="H10" s="60">
+        <v>0</v>
+      </c>
+      <c r="I10" s="60">
+        <v>0</v>
+      </c>
+      <c r="J10" s="60">
+        <v>0</v>
+      </c>
+      <c r="K10" s="60">
+        <v>0</v>
+      </c>
+      <c r="L10" s="61">
+        <v>0</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="69">
+        <v>0</v>
+      </c>
+      <c r="O10" s="97">
+        <f t="array" ref="O10">MMULT(C10:L10,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="59">
+        <v>0</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0</v>
+      </c>
+      <c r="E11" s="60">
+        <v>0</v>
+      </c>
+      <c r="F11" s="60">
+        <v>0</v>
+      </c>
+      <c r="G11" s="60">
+        <v>0</v>
+      </c>
+      <c r="H11" s="60">
+        <v>0</v>
+      </c>
+      <c r="I11" s="60">
+        <v>0</v>
+      </c>
+      <c r="J11" s="60">
+        <v>0</v>
+      </c>
+      <c r="K11" s="60">
+        <v>0</v>
+      </c>
+      <c r="L11" s="61">
+        <v>0</v>
+      </c>
+      <c r="M11" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="69">
+        <v>0</v>
+      </c>
+      <c r="O11" s="97">
+        <f t="array" ref="O11">MMULT(C11:L11,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="59">
+        <v>0</v>
+      </c>
+      <c r="D12" s="60">
+        <v>0</v>
+      </c>
+      <c r="E12" s="60">
+        <v>0</v>
+      </c>
+      <c r="F12" s="60">
+        <v>0</v>
+      </c>
+      <c r="G12" s="60">
+        <v>0</v>
+      </c>
+      <c r="H12" s="60">
+        <v>0</v>
+      </c>
+      <c r="I12" s="60">
+        <v>0</v>
+      </c>
+      <c r="J12" s="60">
+        <v>0</v>
+      </c>
+      <c r="K12" s="60">
+        <v>0</v>
+      </c>
+      <c r="L12" s="61">
+        <v>0</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="69">
+        <v>0</v>
+      </c>
+      <c r="O12" s="97">
+        <f t="array" ref="O12">MMULT(C12:L12,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="126"/>
+      <c r="B13" s="127"/>
+      <c r="C13" s="100">
+        <v>0</v>
+      </c>
+      <c r="D13" s="101">
+        <v>0</v>
+      </c>
+      <c r="E13" s="101">
+        <v>0</v>
+      </c>
+      <c r="F13" s="101">
+        <v>0</v>
+      </c>
+      <c r="G13" s="101">
+        <v>0</v>
+      </c>
+      <c r="H13" s="101">
+        <v>0</v>
+      </c>
+      <c r="I13" s="101">
+        <v>0</v>
+      </c>
+      <c r="J13" s="101">
+        <v>0</v>
+      </c>
+      <c r="K13" s="101">
+        <v>0</v>
+      </c>
+      <c r="L13" s="102">
+        <v>0</v>
+      </c>
+      <c r="M13" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="104">
+        <v>0</v>
+      </c>
+      <c r="O13" s="105">
+        <f t="array" ref="O13">MMULT(C13:L13,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="172" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="177"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="177"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="177"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="177"/>
+      <c r="N15" s="173"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="178"/>
+      <c r="B16" s="179"/>
+      <c r="C16" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="47"/>
+      <c r="N16" s="46"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="172" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="173"/>
+      <c r="C17" s="74">
+        <v>10</v>
+      </c>
+      <c r="D17" s="75">
+        <v>9</v>
+      </c>
+      <c r="E17" s="75">
+        <v>6</v>
+      </c>
+      <c r="F17" s="75">
+        <v>4</v>
+      </c>
+      <c r="G17" s="75">
+        <v>3</v>
+      </c>
+      <c r="H17" s="75">
+        <v>2</v>
+      </c>
+      <c r="I17" s="75">
+        <v>0</v>
+      </c>
+      <c r="J17" s="75">
+        <v>0</v>
+      </c>
+      <c r="K17" s="75">
+        <v>0</v>
+      </c>
+      <c r="L17" s="76">
+        <v>0</v>
+      </c>
+      <c r="M17" s="52"/>
+      <c r="N17" s="49"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="174"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="52"/>
+      <c r="N18" s="54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="172" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="173"/>
+      <c r="C19" s="85">
+        <v>1</v>
+      </c>
+      <c r="D19" s="86">
+        <v>1</v>
+      </c>
+      <c r="E19" s="86">
+        <v>1</v>
+      </c>
+      <c r="F19" s="86">
+        <v>0</v>
+      </c>
+      <c r="G19" s="86">
+        <v>1</v>
+      </c>
+      <c r="H19" s="86">
+        <v>0</v>
+      </c>
+      <c r="I19" s="86">
+        <v>0</v>
+      </c>
+      <c r="J19" s="86">
+        <v>0</v>
+      </c>
+      <c r="K19" s="86">
+        <v>0</v>
+      </c>
+      <c r="L19" s="87">
+        <v>0</v>
+      </c>
+      <c r="M19" s="53"/>
+      <c r="N19" s="88">
+        <f t="array" ref="N19">MMULT(C17:L17,TRANSPOSE(C$19:L$19))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C3:L13">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:L17 C19:L19">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N13">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3F4C55-080C-4628-A564-F2DDFB252D48}">
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="41" customWidth="1"/>
+    <col min="3" max="12" width="9" style="41"/>
+    <col min="13" max="13" width="2.625" style="41" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="41" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="168"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="176" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="173"/>
+      <c r="C2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="195">
+        <v>2</v>
+      </c>
+      <c r="D3" s="196">
+        <v>1</v>
+      </c>
+      <c r="E3" s="196">
+        <v>3</v>
+      </c>
+      <c r="F3" s="196">
+        <v>3</v>
+      </c>
+      <c r="G3" s="196">
+        <v>2</v>
+      </c>
+      <c r="H3" s="196">
+        <v>1</v>
+      </c>
+      <c r="I3" s="196">
+        <v>0</v>
+      </c>
+      <c r="J3" s="196">
+        <v>0</v>
+      </c>
+      <c r="K3" s="196">
+        <v>0</v>
+      </c>
+      <c r="L3" s="197">
+        <v>0</v>
+      </c>
+      <c r="M3" s="198" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="199">
+        <v>8</v>
+      </c>
+      <c r="O3" s="200">
+        <f t="array" ref="O3">MMULT(C3:L3,TRANSPOSE(C$9:L$9))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="172" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="173"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="178"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="47"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="172" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="173"/>
+      <c r="C7" s="74">
+        <v>10</v>
+      </c>
+      <c r="D7" s="75">
+        <v>9</v>
+      </c>
+      <c r="E7" s="75">
+        <v>6</v>
+      </c>
+      <c r="F7" s="75">
+        <v>4</v>
+      </c>
+      <c r="G7" s="75">
+        <v>3</v>
+      </c>
+      <c r="H7" s="75">
+        <v>2</v>
+      </c>
+      <c r="I7" s="75">
+        <v>0</v>
+      </c>
+      <c r="J7" s="75">
+        <v>0</v>
+      </c>
+      <c r="K7" s="75">
+        <v>0</v>
+      </c>
+      <c r="L7" s="76">
+        <v>0</v>
+      </c>
+      <c r="M7" s="52"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="174"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="52"/>
+      <c r="N8" s="54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="172" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="173"/>
+      <c r="C9" s="85">
+        <v>1</v>
+      </c>
+      <c r="D9" s="86">
+        <v>1</v>
+      </c>
+      <c r="E9" s="86">
+        <v>1</v>
+      </c>
+      <c r="F9" s="86">
+        <v>0</v>
+      </c>
+      <c r="G9" s="86">
+        <v>1</v>
+      </c>
+      <c r="H9" s="86">
+        <v>0</v>
+      </c>
+      <c r="I9" s="86">
+        <v>0</v>
+      </c>
+      <c r="J9" s="86">
+        <v>0</v>
+      </c>
+      <c r="K9" s="86">
+        <v>0</v>
+      </c>
+      <c r="L9" s="87">
+        <v>0</v>
+      </c>
+      <c r="M9" s="53"/>
+      <c r="N9" s="88">
+        <f t="array" ref="N9">MMULT(C7:L7,TRANSPOSE(C$9:L$9))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C3:L3">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:L7 C9:L9">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BE7343-A42A-4384-8199-E4067600D7F0}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.625" style="148" customWidth="1"/>
+    <col min="2" max="3" width="4.625" style="149" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="150" customWidth="1"/>
+    <col min="5" max="5" width="2.625" customWidth="1"/>
+    <col min="6" max="7" width="4.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.625" customWidth="1"/>
+    <col min="9" max="9" width="4.625" style="153" customWidth="1"/>
+    <col min="10" max="11" width="4.625" style="154" customWidth="1"/>
+    <col min="12" max="12" width="8.625" style="155" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="156" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="157" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="150" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="172" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="194"/>
+      <c r="I1" s="201" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="193"/>
+      <c r="M1" s="193"/>
+      <c r="N1" s="193"/>
+      <c r="O1" s="194"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="147" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="144" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="147" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="202" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="158">
+        <v>1</v>
+      </c>
+      <c r="B3" s="159">
+        <v>4</v>
+      </c>
+      <c r="C3" s="159">
+        <v>3</v>
+      </c>
+      <c r="D3" s="160">
+        <f>B3/C3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F3" s="151">
+        <v>5</v>
+      </c>
+      <c r="G3" s="152">
+        <v>6</v>
+      </c>
+      <c r="I3" s="161">
+        <v>2</v>
+      </c>
+      <c r="J3" s="162">
+        <v>2</v>
+      </c>
+      <c r="K3" s="162">
+        <v>1</v>
+      </c>
+      <c r="L3" s="163">
+        <f>J3/K3</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="164">
+        <f>G3-K3</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="165">
+        <f>SUM(J$3:J3)</f>
+        <v>2</v>
+      </c>
+      <c r="O3" s="160">
+        <f>IF(M3&gt;=0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="148">
+        <v>2</v>
+      </c>
+      <c r="B4" s="149">
+        <v>2</v>
+      </c>
+      <c r="C4" s="149">
+        <v>1</v>
+      </c>
+      <c r="D4" s="150">
+        <f>B4/C4</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="153">
+        <v>4</v>
+      </c>
+      <c r="J4" s="154">
+        <v>5</v>
+      </c>
+      <c r="K4" s="154">
+        <v>3</v>
+      </c>
+      <c r="L4" s="155">
+        <f>J4/K4</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M4" s="156">
+        <f>M3-K4</f>
+        <v>2</v>
+      </c>
+      <c r="N4" s="157">
+        <f>SUM(J$3:J4)</f>
+        <v>7</v>
+      </c>
+      <c r="O4" s="150">
+        <f t="shared" ref="O4:O7" si="0">IF(M4&gt;=0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="148">
+        <v>3</v>
+      </c>
+      <c r="B5" s="149">
+        <v>3</v>
+      </c>
+      <c r="C5" s="149">
+        <v>2</v>
+      </c>
+      <c r="D5" s="150">
+        <f>B5/C5</f>
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="153">
+        <v>3</v>
+      </c>
+      <c r="J5" s="154">
+        <v>3</v>
+      </c>
+      <c r="K5" s="154">
+        <v>2</v>
+      </c>
+      <c r="L5" s="155">
+        <f>J5/K5</f>
+        <v>1.5</v>
+      </c>
+      <c r="M5" s="156">
+        <f t="shared" ref="M5:M7" si="1">M4-K5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="157">
+        <f>SUM(J$3:J5)</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="150">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="148">
+        <v>4</v>
+      </c>
+      <c r="B6" s="149">
+        <v>5</v>
+      </c>
+      <c r="C6" s="149">
+        <v>3</v>
+      </c>
+      <c r="D6" s="150">
+        <f>B6/C6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I6" s="153">
+        <v>1</v>
+      </c>
+      <c r="J6" s="154">
+        <v>4</v>
+      </c>
+      <c r="K6" s="154">
+        <v>3</v>
+      </c>
+      <c r="L6" s="155">
+        <f>J6/K6</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="M6" s="156">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="N6" s="157">
+        <f>SUM(J$3:J6)</f>
+        <v>14</v>
+      </c>
+      <c r="O6" s="150">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="148">
+        <v>5</v>
+      </c>
+      <c r="B7" s="149">
+        <v>1</v>
+      </c>
+      <c r="C7" s="149">
+        <v>1</v>
+      </c>
+      <c r="D7" s="150">
+        <f>B7/C7</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="153">
+        <v>5</v>
+      </c>
+      <c r="J7" s="154">
+        <v>1</v>
+      </c>
+      <c r="K7" s="154">
+        <v>1</v>
+      </c>
+      <c r="L7" s="155">
+        <f>J7/K7</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="156">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="N7" s="157">
+        <f>SUM(J$3:J7)</f>
+        <v>15</v>
+      </c>
+      <c r="O7" s="150">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rearrange LP and CO excel
</commit_message>
<xml_diff>
--- a/_Excel/LP.xlsx
+++ b/_Excel/LP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bridge\City2223_SEM_A\EE3301\letcure\edit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bridge\City2223_SEM_A\EE3301\letcure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A9096D-6411-4D0B-81AA-6BBE23C6588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C88D0B1-0A89-41C1-B904-5F28D33ACE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" xr2:uid="{DA5D110B-5606-4367-BCF8-9589C927E560}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" activeTab="7" xr2:uid="{DA5D110B-5606-4367-BCF8-9589C927E560}"/>
   </bookViews>
   <sheets>
     <sheet name="LP" sheetId="1" r:id="rId1"/>
@@ -18,181 +18,266 @@
     <sheet name="LP Mat" sheetId="4" r:id="rId3"/>
     <sheet name="LP Mat UV" sheetId="5" r:id="rId4"/>
     <sheet name="Dual" sheetId="6" r:id="rId5"/>
+    <sheet name="Knapsack LP" sheetId="7" r:id="rId6"/>
+    <sheet name="Knapsack ILP" sheetId="8" r:id="rId7"/>
+    <sheet name="Knapsack Greedy" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="4" hidden="1">Dual!$C$39:$L$39</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'Knapsack ILP'!$C$9:$L$9</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'Knapsack LP'!$C$19:$L$19</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">LP!$E$11:$G$11</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'LP Mat'!$C$23:$L$23</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'LP Mat UV'!$C$23:$L$24</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'LP UV'!$E$11:$K$11</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs0" localSheetId="6" hidden="1">'Knapsack ILP'!$O$3:$O$3</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">Dual!$O$24:$O$33</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Knapsack ILP'!$O$3</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Knapsack LP'!$C$19:$L$19</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">LP!$F$3:$F$7</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'LP Mat'!$C$23:$L$23</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'LP Mat UV'!$O$13:$O$17</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'LP UV'!$F$3:$F$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'Knapsack ILP'!$C$9:$L$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Knapsack LP'!$O$3:$O$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">LP!$M$3:$M$7</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'LP Mat'!$O$13:$O$17</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'LP Mat UV'!$O$3:$O$7</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'LP UV'!$M$3:$M$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">'Knapsack ILP'!$O$3:$O$3</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">LP!$M$3:$M$7</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'LP Mat'!$O$3:$O$7</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'LP Mat UV'!$O$8:$O$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="6" hidden="1">'Knapsack ILP'!#REF!</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'LP Mat'!$O$8:$O$12</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'LP Mat'!$O$9:$O$13</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">Dual!$N$39</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Knapsack Greedy'!$N$19</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'Knapsack ILP'!$N$9</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'Knapsack LP'!$N$19</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">LP!$H$11</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'LP Mat'!$N$23</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'LP Mat UV'!$N$23</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'LP UV'!$L$11</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel0" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs0" localSheetId="6" hidden="1">'Knapsack ILP'!$N$3:$N$3</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">Dual!$N$24:$N$33</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">'Knapsack ILP'!$N$3</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">"整數"</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">LP!$E$3:$E$7</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">"整數"</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">'LP Mat UV'!$N$13:$N$17</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'LP UV'!$E$3:$E$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">"二進制"</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">'Knapsack LP'!$N$3:$N$13</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">LP!$L$3:$L$7</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'LP Mat'!$N$13:$N$17</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">'LP Mat UV'!$N$3:$N$7</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'LP UV'!$L$3:$L$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="6" hidden="1">'Knapsack ILP'!$N$3:$N$3</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">LP!$L$3:$L$7</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'LP Mat'!$N$3:$N$7</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">'LP Mat UV'!$N$8:$N$12</definedName>
+    <definedName name="solver_rhs4" localSheetId="6" hidden="1">'Knapsack ILP'!#REF!</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'LP Mat'!$N$8:$N$12</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">'LP Mat'!$N$9:$N$13</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
@@ -216,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="85">
   <si>
     <t>Subject to</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -490,12 +575,78 @@
     <t>Diff</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>P function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>W remain</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi/wi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (You need to sort the table by yourself)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unsort</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -555,6 +706,14 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -594,7 +753,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="86">
+  <borders count="92">
     <border>
       <left/>
       <right/>
@@ -1705,13 +1864,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2123,6 +2362,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2174,6 +2422,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2189,17 +2443,150 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="89" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="90" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="89" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="91" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="90" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="91" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="90" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2597,7 +2984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AD5AAE-0753-4E18-8CF1-18AD53E0EAE9}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -2608,21 +2995,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="139"/>
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="142"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -2810,16 +3197,16 @@
     </row>
     <row r="8" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="141"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="142"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="144"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="145"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -2895,21 +3282,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="139"/>
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="142"/>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -3101,24 +3488,24 @@
     </row>
     <row r="8" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="141"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="141"/>
-      <c r="J9" s="141"/>
-      <c r="K9" s="141"/>
-      <c r="L9" s="141"/>
-      <c r="M9" s="141"/>
-      <c r="N9" s="141"/>
-      <c r="O9" s="141"/>
-      <c r="P9" s="142"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="144"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="144"/>
+      <c r="J9" s="144"/>
+      <c r="K9" s="144"/>
+      <c r="L9" s="144"/>
+      <c r="M9" s="144"/>
+      <c r="N9" s="144"/>
+      <c r="O9" s="144"/>
+      <c r="P9" s="145"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -3246,29 +3633,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="139"/>
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="142"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="144"/>
+      <c r="B2" s="147"/>
       <c r="C2" s="41" t="s">
         <v>8</v>
       </c>
@@ -3967,26 +4354,26 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
-      <c r="K19" s="148"/>
-      <c r="L19" s="148"/>
-      <c r="M19" s="148"/>
-      <c r="N19" s="144"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="151"/>
+      <c r="N19" s="147"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="149"/>
-      <c r="B20" s="150"/>
+      <c r="A20" s="152"/>
+      <c r="B20" s="153"/>
       <c r="C20" s="45" t="s">
         <v>47</v>
       </c>
@@ -4021,10 +4408,10 @@
       <c r="N20" s="46"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="144"/>
+      <c r="B21" s="147"/>
       <c r="C21" s="74">
         <v>4</v>
       </c>
@@ -4059,8 +4446,8 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="145"/>
-      <c r="B22" s="146"/>
+      <c r="A22" s="148"/>
+      <c r="B22" s="149"/>
       <c r="C22" s="41" t="s">
         <v>8</v>
       </c>
@@ -4097,10 +4484,10 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="144"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="85">
         <v>0</v>
       </c>
@@ -4197,17 +4584,17 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:L17">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21 C23:L23">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4235,29 +4622,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="139"/>
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="142"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="150"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="41" t="s">
         <v>8</v>
       </c>
@@ -4956,26 +5343,26 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
-      <c r="K19" s="148"/>
-      <c r="L19" s="148"/>
-      <c r="M19" s="148"/>
-      <c r="N19" s="144"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="151"/>
+      <c r="N19" s="147"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="149"/>
-      <c r="B20" s="150"/>
+      <c r="A20" s="152"/>
+      <c r="B20" s="153"/>
       <c r="C20" s="45" t="s">
         <v>47</v>
       </c>
@@ -5010,10 +5397,10 @@
       <c r="N20" s="49"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="144"/>
+      <c r="B21" s="147"/>
       <c r="C21" s="74">
         <v>7</v>
       </c>
@@ -5048,8 +5435,8 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="145"/>
-      <c r="B22" s="146"/>
+      <c r="A22" s="148"/>
+      <c r="B22" s="149"/>
       <c r="C22" s="42" t="s">
         <v>8</v>
       </c>
@@ -5086,10 +5473,10 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="149" t="s">
+      <c r="A23" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="150"/>
+      <c r="B23" s="153"/>
       <c r="C23" s="77">
         <v>5</v>
       </c>
@@ -5127,10 +5514,10 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="151" t="s">
+      <c r="A24" s="154" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="152"/>
+      <c r="B24" s="155"/>
       <c r="C24" s="81">
         <v>0</v>
       </c>
@@ -5177,12 +5564,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:L17 C21:L21 C23:L24">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N17">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5214,48 +5601,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
-      <c r="O1" s="155"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
+      <c r="O1" s="160"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="139"/>
+      <c r="A2" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141"/>
+      <c r="O2" s="142"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="144"/>
+      <c r="B3" s="147"/>
       <c r="C3" s="41" t="s">
         <v>8</v>
       </c>
@@ -5734,26 +6121,26 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="143" t="s">
+      <c r="A15" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="148"/>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-      <c r="L15" s="148"/>
-      <c r="M15" s="148"/>
-      <c r="N15" s="144"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="147"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="144"/>
+      <c r="A16" s="146"/>
+      <c r="B16" s="147"/>
       <c r="C16" s="45" t="s">
         <v>47</v>
       </c>
@@ -5788,10 +6175,10 @@
       <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="144"/>
+      <c r="B17" s="147"/>
       <c r="C17" s="74">
         <v>4.2999999999999997E-2</v>
       </c>
@@ -5826,8 +6213,8 @@
       <c r="N17" s="49"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="144"/>
+      <c r="A18" s="146"/>
+      <c r="B18" s="147"/>
       <c r="C18" s="41" t="s">
         <v>8</v>
       </c>
@@ -5864,10 +6251,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="144"/>
+      <c r="B19" s="147"/>
       <c r="C19" s="85">
         <v>2.1818181818181817</v>
       </c>
@@ -5921,48 +6308,48 @@
       <c r="N20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
-      <c r="L21" s="157"/>
-      <c r="M21" s="157"/>
-      <c r="N21" s="157"/>
-      <c r="O21" s="158"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="162"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="162"/>
+      <c r="I21" s="162"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="162"/>
+      <c r="L21" s="162"/>
+      <c r="M21" s="162"/>
+      <c r="N21" s="162"/>
+      <c r="O21" s="163"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="138"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="J22" s="138"/>
-      <c r="K22" s="138"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="138"/>
-      <c r="N22" s="138"/>
-      <c r="O22" s="139"/>
+      <c r="A22" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="141"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="141"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="141"/>
+      <c r="J22" s="141"/>
+      <c r="K22" s="141"/>
+      <c r="L22" s="141"/>
+      <c r="M22" s="141"/>
+      <c r="N22" s="141"/>
+      <c r="O22" s="142"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="147" t="s">
+      <c r="A23" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="144"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="41" t="s">
         <v>58</v>
       </c>
@@ -6444,27 +6831,27 @@
     </row>
     <row r="34" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="137" t="s">
+      <c r="A35" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="138"/>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="138"/>
-      <c r="I35" s="138"/>
-      <c r="J35" s="138"/>
-      <c r="K35" s="138"/>
-      <c r="L35" s="138"/>
-      <c r="M35" s="138"/>
-      <c r="N35" s="138"/>
-      <c r="O35" s="139"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="141"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="141"/>
+      <c r="H35" s="141"/>
+      <c r="I35" s="141"/>
+      <c r="J35" s="141"/>
+      <c r="K35" s="141"/>
+      <c r="L35" s="141"/>
+      <c r="M35" s="141"/>
+      <c r="N35" s="141"/>
+      <c r="O35" s="142"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="147"/>
-      <c r="B36" s="144"/>
+      <c r="A36" s="150"/>
+      <c r="B36" s="147"/>
       <c r="C36" s="45" t="s">
         <v>30</v>
       </c>
@@ -6500,10 +6887,10 @@
       <c r="O36" s="128"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="147" t="s">
+      <c r="A37" s="150" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="144"/>
+      <c r="B37" s="147"/>
       <c r="C37" s="85">
         <f t="array" ref="C37:L37">TRANSPOSE(N4:N13)</f>
         <v>10</v>
@@ -6540,8 +6927,8 @@
       <c r="O37" s="129"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="147"/>
-      <c r="B38" s="144"/>
+      <c r="A38" s="150"/>
+      <c r="B38" s="147"/>
       <c r="C38" s="41" t="s">
         <v>58</v>
       </c>
@@ -6581,10 +6968,10 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="159" t="s">
+      <c r="A39" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="160"/>
+      <c r="B39" s="158"/>
       <c r="C39" s="130">
         <v>2.9836363636363637E-2</v>
       </c>
@@ -6627,6 +7014,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:O22"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A17:B17"/>
@@ -6638,43 +7030,1522 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A21:O21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:O22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C4:L13">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:L17 C19:L19">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:L37 C39:L39">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:L33">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N13">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N24:N33">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A743DBBB-AD50-4AC5-A298-F63470BF782B}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="41" customWidth="1"/>
+    <col min="3" max="12" width="9" style="41"/>
+    <col min="13" max="13" width="2.625" style="41" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="41" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="142"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="150" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="147"/>
+      <c r="C2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="91" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="120"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="56">
+        <v>2</v>
+      </c>
+      <c r="D3" s="57">
+        <v>1</v>
+      </c>
+      <c r="E3" s="57">
+        <v>3</v>
+      </c>
+      <c r="F3" s="57">
+        <v>3</v>
+      </c>
+      <c r="G3" s="57">
+        <v>2</v>
+      </c>
+      <c r="H3" s="57">
+        <v>1</v>
+      </c>
+      <c r="I3" s="57">
+        <v>0</v>
+      </c>
+      <c r="J3" s="57">
+        <v>0</v>
+      </c>
+      <c r="K3" s="57">
+        <v>0</v>
+      </c>
+      <c r="L3" s="58">
+        <v>0</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="68">
+        <v>8</v>
+      </c>
+      <c r="O3" s="93">
+        <f t="array" ref="O3">MMULT(C3:L3,TRANSPOSE(C$19:L$19))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="59">
+        <v>1</v>
+      </c>
+      <c r="D4" s="60">
+        <v>0</v>
+      </c>
+      <c r="E4" s="60">
+        <v>0</v>
+      </c>
+      <c r="F4" s="60">
+        <v>0</v>
+      </c>
+      <c r="G4" s="60">
+        <v>0</v>
+      </c>
+      <c r="H4" s="60">
+        <v>0</v>
+      </c>
+      <c r="I4" s="60">
+        <v>0</v>
+      </c>
+      <c r="J4" s="60">
+        <v>0</v>
+      </c>
+      <c r="K4" s="60">
+        <v>0</v>
+      </c>
+      <c r="L4" s="61">
+        <v>0</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="69">
+        <v>1</v>
+      </c>
+      <c r="O4" s="95">
+        <f t="array" ref="O4">MMULT(C4:L4,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="59">
+        <v>0</v>
+      </c>
+      <c r="D5" s="60">
+        <v>1</v>
+      </c>
+      <c r="E5" s="60">
+        <v>0</v>
+      </c>
+      <c r="F5" s="60">
+        <v>0</v>
+      </c>
+      <c r="G5" s="60">
+        <v>0</v>
+      </c>
+      <c r="H5" s="60">
+        <v>0</v>
+      </c>
+      <c r="I5" s="60">
+        <v>0</v>
+      </c>
+      <c r="J5" s="60">
+        <v>0</v>
+      </c>
+      <c r="K5" s="60">
+        <v>0</v>
+      </c>
+      <c r="L5" s="61">
+        <v>0</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="69">
+        <v>1</v>
+      </c>
+      <c r="O5" s="95">
+        <f t="array" ref="O5">MMULT(C5:L5,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="59">
+        <v>0</v>
+      </c>
+      <c r="D6" s="60">
+        <v>0</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="F6" s="60">
+        <v>0</v>
+      </c>
+      <c r="G6" s="60">
+        <v>0</v>
+      </c>
+      <c r="H6" s="60">
+        <v>0</v>
+      </c>
+      <c r="I6" s="60">
+        <v>0</v>
+      </c>
+      <c r="J6" s="60">
+        <v>0</v>
+      </c>
+      <c r="K6" s="60">
+        <v>0</v>
+      </c>
+      <c r="L6" s="61">
+        <v>0</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="69">
+        <v>1</v>
+      </c>
+      <c r="O6" s="95">
+        <f t="array" ref="O6">MMULT(C6:L6,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="59">
+        <v>0</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0</v>
+      </c>
+      <c r="E7" s="60">
+        <v>0</v>
+      </c>
+      <c r="F7" s="60">
+        <v>1</v>
+      </c>
+      <c r="G7" s="60">
+        <v>0</v>
+      </c>
+      <c r="H7" s="60">
+        <v>0</v>
+      </c>
+      <c r="I7" s="60">
+        <v>0</v>
+      </c>
+      <c r="J7" s="60">
+        <v>0</v>
+      </c>
+      <c r="K7" s="60">
+        <v>0</v>
+      </c>
+      <c r="L7" s="61">
+        <v>0</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="69">
+        <v>1</v>
+      </c>
+      <c r="O7" s="95">
+        <f t="array" ref="O7">MMULT(C7:L7,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="59">
+        <v>0</v>
+      </c>
+      <c r="D8" s="60">
+        <v>0</v>
+      </c>
+      <c r="E8" s="60">
+        <v>0</v>
+      </c>
+      <c r="F8" s="60">
+        <v>0</v>
+      </c>
+      <c r="G8" s="60">
+        <v>1</v>
+      </c>
+      <c r="H8" s="60">
+        <v>0</v>
+      </c>
+      <c r="I8" s="60">
+        <v>0</v>
+      </c>
+      <c r="J8" s="60">
+        <v>0</v>
+      </c>
+      <c r="K8" s="60">
+        <v>0</v>
+      </c>
+      <c r="L8" s="61">
+        <v>0</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="69">
+        <v>1</v>
+      </c>
+      <c r="O8" s="95">
+        <f t="array" ref="O8">MMULT(C8:L8,TRANSPOSE(C$19:L$19))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="59">
+        <v>0</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0</v>
+      </c>
+      <c r="E9" s="60">
+        <v>0</v>
+      </c>
+      <c r="F9" s="60">
+        <v>0</v>
+      </c>
+      <c r="G9" s="60">
+        <v>0</v>
+      </c>
+      <c r="H9" s="60">
+        <v>1</v>
+      </c>
+      <c r="I9" s="60">
+        <v>0</v>
+      </c>
+      <c r="J9" s="60">
+        <v>0</v>
+      </c>
+      <c r="K9" s="60">
+        <v>0</v>
+      </c>
+      <c r="L9" s="61">
+        <v>0</v>
+      </c>
+      <c r="M9" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="69">
+        <v>1</v>
+      </c>
+      <c r="O9" s="95">
+        <f t="array" ref="O9">MMULT(C9:L9,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="59">
+        <v>0</v>
+      </c>
+      <c r="D10" s="60">
+        <v>0</v>
+      </c>
+      <c r="E10" s="60">
+        <v>0</v>
+      </c>
+      <c r="F10" s="60">
+        <v>0</v>
+      </c>
+      <c r="G10" s="60">
+        <v>0</v>
+      </c>
+      <c r="H10" s="60">
+        <v>0</v>
+      </c>
+      <c r="I10" s="60">
+        <v>0</v>
+      </c>
+      <c r="J10" s="60">
+        <v>0</v>
+      </c>
+      <c r="K10" s="60">
+        <v>0</v>
+      </c>
+      <c r="L10" s="61">
+        <v>0</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="69">
+        <v>0</v>
+      </c>
+      <c r="O10" s="95">
+        <f t="array" ref="O10">MMULT(C10:L10,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="59">
+        <v>0</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0</v>
+      </c>
+      <c r="E11" s="60">
+        <v>0</v>
+      </c>
+      <c r="F11" s="60">
+        <v>0</v>
+      </c>
+      <c r="G11" s="60">
+        <v>0</v>
+      </c>
+      <c r="H11" s="60">
+        <v>0</v>
+      </c>
+      <c r="I11" s="60">
+        <v>0</v>
+      </c>
+      <c r="J11" s="60">
+        <v>0</v>
+      </c>
+      <c r="K11" s="60">
+        <v>0</v>
+      </c>
+      <c r="L11" s="61">
+        <v>0</v>
+      </c>
+      <c r="M11" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="69">
+        <v>0</v>
+      </c>
+      <c r="O11" s="95">
+        <f t="array" ref="O11">MMULT(C11:L11,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="59">
+        <v>0</v>
+      </c>
+      <c r="D12" s="60">
+        <v>0</v>
+      </c>
+      <c r="E12" s="60">
+        <v>0</v>
+      </c>
+      <c r="F12" s="60">
+        <v>0</v>
+      </c>
+      <c r="G12" s="60">
+        <v>0</v>
+      </c>
+      <c r="H12" s="60">
+        <v>0</v>
+      </c>
+      <c r="I12" s="60">
+        <v>0</v>
+      </c>
+      <c r="J12" s="60">
+        <v>0</v>
+      </c>
+      <c r="K12" s="60">
+        <v>0</v>
+      </c>
+      <c r="L12" s="61">
+        <v>0</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="69">
+        <v>0</v>
+      </c>
+      <c r="O12" s="95">
+        <f t="array" ref="O12">MMULT(C12:L12,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="124"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="98">
+        <v>0</v>
+      </c>
+      <c r="D13" s="99">
+        <v>0</v>
+      </c>
+      <c r="E13" s="99">
+        <v>0</v>
+      </c>
+      <c r="F13" s="99">
+        <v>0</v>
+      </c>
+      <c r="G13" s="99">
+        <v>0</v>
+      </c>
+      <c r="H13" s="99">
+        <v>0</v>
+      </c>
+      <c r="I13" s="99">
+        <v>0</v>
+      </c>
+      <c r="J13" s="99">
+        <v>0</v>
+      </c>
+      <c r="K13" s="99">
+        <v>0</v>
+      </c>
+      <c r="L13" s="100">
+        <v>0</v>
+      </c>
+      <c r="M13" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="102">
+        <v>0</v>
+      </c>
+      <c r="O13" s="103">
+        <f t="array" ref="O13">MMULT(C13:L13,TRANSPOSE(C$19:L$19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="147"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="152"/>
+      <c r="B16" s="153"/>
+      <c r="C16" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="47"/>
+      <c r="N16" s="46"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="146" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="147"/>
+      <c r="C17" s="74">
+        <v>10</v>
+      </c>
+      <c r="D17" s="75">
+        <v>9</v>
+      </c>
+      <c r="E17" s="75">
+        <v>6</v>
+      </c>
+      <c r="F17" s="75">
+        <v>4</v>
+      </c>
+      <c r="G17" s="75">
+        <v>3</v>
+      </c>
+      <c r="H17" s="75">
+        <v>2</v>
+      </c>
+      <c r="I17" s="75">
+        <v>0</v>
+      </c>
+      <c r="J17" s="75">
+        <v>0</v>
+      </c>
+      <c r="K17" s="75">
+        <v>0</v>
+      </c>
+      <c r="L17" s="76">
+        <v>0</v>
+      </c>
+      <c r="M17" s="52"/>
+      <c r="N17" s="49"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="148"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="52"/>
+      <c r="N18" s="54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="146" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="147"/>
+      <c r="C19" s="85">
+        <v>1</v>
+      </c>
+      <c r="D19" s="86">
+        <v>1</v>
+      </c>
+      <c r="E19" s="86">
+        <v>1</v>
+      </c>
+      <c r="F19" s="86">
+        <v>0</v>
+      </c>
+      <c r="G19" s="86">
+        <v>1</v>
+      </c>
+      <c r="H19" s="86">
+        <v>0</v>
+      </c>
+      <c r="I19" s="86">
+        <v>0</v>
+      </c>
+      <c r="J19" s="86">
+        <v>0</v>
+      </c>
+      <c r="K19" s="86">
+        <v>0</v>
+      </c>
+      <c r="L19" s="87">
+        <v>0</v>
+      </c>
+      <c r="M19" s="53"/>
+      <c r="N19" s="88">
+        <f t="array" ref="N19">MMULT(C17:L17,TRANSPOSE(C$19:L$19))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C3:L13">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:L17 C19:L19">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N13">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B83F50B-525F-4597-9782-53C7EF59589E}">
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="41" customWidth="1"/>
+    <col min="3" max="12" width="9" style="41"/>
+    <col min="13" max="13" width="2.625" style="41" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="41" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="142"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="150" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="147"/>
+      <c r="C2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="91" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="138"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="169">
+        <v>2</v>
+      </c>
+      <c r="D3" s="168">
+        <v>1</v>
+      </c>
+      <c r="E3" s="168">
+        <v>3</v>
+      </c>
+      <c r="F3" s="168">
+        <v>3</v>
+      </c>
+      <c r="G3" s="168">
+        <v>2</v>
+      </c>
+      <c r="H3" s="168">
+        <v>1</v>
+      </c>
+      <c r="I3" s="168">
+        <v>0</v>
+      </c>
+      <c r="J3" s="168">
+        <v>0</v>
+      </c>
+      <c r="K3" s="168">
+        <v>0</v>
+      </c>
+      <c r="L3" s="167">
+        <v>0</v>
+      </c>
+      <c r="M3" s="166" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="165">
+        <v>8</v>
+      </c>
+      <c r="O3" s="164">
+        <f t="array" ref="O3">MMULT(C3:L3,TRANSPOSE(C$9:L$9))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="151"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
+      <c r="I5" s="151"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151"/>
+      <c r="L5" s="151"/>
+      <c r="M5" s="151"/>
+      <c r="N5" s="147"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="152"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="47"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="146" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="147"/>
+      <c r="C7" s="74">
+        <v>10</v>
+      </c>
+      <c r="D7" s="75">
+        <v>9</v>
+      </c>
+      <c r="E7" s="75">
+        <v>6</v>
+      </c>
+      <c r="F7" s="75">
+        <v>4</v>
+      </c>
+      <c r="G7" s="75">
+        <v>3</v>
+      </c>
+      <c r="H7" s="75">
+        <v>2</v>
+      </c>
+      <c r="I7" s="75">
+        <v>0</v>
+      </c>
+      <c r="J7" s="75">
+        <v>0</v>
+      </c>
+      <c r="K7" s="75">
+        <v>0</v>
+      </c>
+      <c r="L7" s="76">
+        <v>0</v>
+      </c>
+      <c r="M7" s="52"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="148"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="52"/>
+      <c r="N8" s="54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="146" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="147"/>
+      <c r="C9" s="85">
+        <v>1</v>
+      </c>
+      <c r="D9" s="86">
+        <v>1</v>
+      </c>
+      <c r="E9" s="86">
+        <v>1</v>
+      </c>
+      <c r="F9" s="86">
+        <v>0</v>
+      </c>
+      <c r="G9" s="86">
+        <v>1</v>
+      </c>
+      <c r="H9" s="86">
+        <v>0</v>
+      </c>
+      <c r="I9" s="86">
+        <v>0</v>
+      </c>
+      <c r="J9" s="86">
+        <v>0</v>
+      </c>
+      <c r="K9" s="86">
+        <v>0</v>
+      </c>
+      <c r="L9" s="87">
+        <v>0</v>
+      </c>
+      <c r="M9" s="53"/>
+      <c r="N9" s="88">
+        <f t="array" ref="N9">MMULT(C7:L7,TRANSPOSE(C$9:L$9))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C3:L3">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N13">
+  <conditionalFormatting sqref="C7:L7 C9:L9">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N24:N33">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B617BD-3248-4AEE-BE28-BA42EC93920B}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.625" style="177" customWidth="1"/>
+    <col min="2" max="3" width="4.625" style="176" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="170" customWidth="1"/>
+    <col min="5" max="5" width="2.625" customWidth="1"/>
+    <col min="6" max="7" width="4.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.625" customWidth="1"/>
+    <col min="9" max="9" width="4.625" style="175" customWidth="1"/>
+    <col min="10" max="11" width="4.625" style="174" customWidth="1"/>
+    <col min="12" max="12" width="8.625" style="173" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="172" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="171" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="170" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="146" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="190"/>
+      <c r="I1" s="192" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="190"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="189" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="137" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="189" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="188" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="187">
+        <v>1</v>
+      </c>
+      <c r="B3" s="186">
+        <v>4</v>
+      </c>
+      <c r="C3" s="186">
+        <v>3</v>
+      </c>
+      <c r="D3" s="178">
+        <f>B3/C3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F3" s="185">
+        <v>5</v>
+      </c>
+      <c r="G3" s="184">
+        <v>6</v>
+      </c>
+      <c r="I3" s="183">
+        <v>2</v>
+      </c>
+      <c r="J3" s="182">
+        <v>2</v>
+      </c>
+      <c r="K3" s="182">
+        <v>1</v>
+      </c>
+      <c r="L3" s="181">
+        <f>J3/K3</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="180">
+        <f>G3-K3</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="179">
+        <f>SUM(J$3:J3)</f>
+        <v>2</v>
+      </c>
+      <c r="O3" s="178">
+        <f>IF(M3&gt;=0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="177">
+        <v>2</v>
+      </c>
+      <c r="B4" s="176">
+        <v>2</v>
+      </c>
+      <c r="C4" s="176">
+        <v>1</v>
+      </c>
+      <c r="D4" s="170">
+        <f>B4/C4</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="175">
+        <v>4</v>
+      </c>
+      <c r="J4" s="174">
+        <v>5</v>
+      </c>
+      <c r="K4" s="174">
+        <v>3</v>
+      </c>
+      <c r="L4" s="173">
+        <f>J4/K4</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M4" s="172">
+        <f>M3-K4</f>
+        <v>2</v>
+      </c>
+      <c r="N4" s="171">
+        <f>SUM(J$3:J4)</f>
+        <v>7</v>
+      </c>
+      <c r="O4" s="170">
+        <f>IF(M4&gt;=0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="177">
+        <v>3</v>
+      </c>
+      <c r="B5" s="176">
+        <v>3</v>
+      </c>
+      <c r="C5" s="176">
+        <v>2</v>
+      </c>
+      <c r="D5" s="170">
+        <f>B5/C5</f>
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="175">
+        <v>3</v>
+      </c>
+      <c r="J5" s="174">
+        <v>3</v>
+      </c>
+      <c r="K5" s="174">
+        <v>2</v>
+      </c>
+      <c r="L5" s="173">
+        <f>J5/K5</f>
+        <v>1.5</v>
+      </c>
+      <c r="M5" s="172">
+        <f>M4-K5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="171">
+        <f>SUM(J$3:J5)</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="170">
+        <f>IF(M5&gt;=0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="177">
+        <v>4</v>
+      </c>
+      <c r="B6" s="176">
+        <v>5</v>
+      </c>
+      <c r="C6" s="176">
+        <v>3</v>
+      </c>
+      <c r="D6" s="170">
+        <f>B6/C6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I6" s="175">
+        <v>1</v>
+      </c>
+      <c r="J6" s="174">
+        <v>4</v>
+      </c>
+      <c r="K6" s="174">
+        <v>3</v>
+      </c>
+      <c r="L6" s="173">
+        <f>J6/K6</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="M6" s="172">
+        <f>M5-K6</f>
+        <v>-3</v>
+      </c>
+      <c r="N6" s="171">
+        <f>SUM(J$3:J6)</f>
+        <v>14</v>
+      </c>
+      <c r="O6" s="170">
+        <f>IF(M6&gt;=0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="177">
+        <v>5</v>
+      </c>
+      <c r="B7" s="176">
+        <v>1</v>
+      </c>
+      <c r="C7" s="176">
+        <v>1</v>
+      </c>
+      <c r="D7" s="170">
+        <f>B7/C7</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="175">
+        <v>5</v>
+      </c>
+      <c r="J7" s="174">
+        <v>1</v>
+      </c>
+      <c r="K7" s="174">
+        <v>1</v>
+      </c>
+      <c r="L7" s="173">
+        <f>J7/K7</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="172">
+        <f>M6-K7</f>
+        <v>-4</v>
+      </c>
+      <c r="N7" s="171">
+        <f>SUM(J$3:J7)</f>
+        <v>15</v>
+      </c>
+      <c r="O7" s="170">
+        <f>IF(M7&gt;=0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>